<commit_message>
Add python entry on array/dict/set basics
</commit_message>
<xml_diff>
--- a/python.xlsx
+++ b/python.xlsx
@@ -16,68 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
-  <si>
-    <t>Conda</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List packages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conda list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conda env list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Move to an env</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(on bash) source activate {env_name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(on bash) source deactivate {env_name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>list environment/ chk out current env</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create an Env</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conda create -n {env_name} {needed_package_1} {needed_package_2}
-e.g. conda create -n my_env numpy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Conda</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Install package</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conda install numpy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>/* move the python 101 here */</t>
   </si>
   <si>
     <t>Pip</t>
-  </si>
-  <si>
-    <t>Python2 vs 3</t>
   </si>
   <si>
     <t>There is big syntax change between 2,3. One significant diff is: 
@@ -91,13 +35,508 @@
     <t>*** prequsition: add …/python27/scripts to cmd path ***
 $ pip search xlrd 
 $ pip install xlrd</t>
+  </si>
+  <si>
+    <t>Conda</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>package basic</t>
+  </si>
+  <si>
+    <t>Environment basic</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Diff of v2 v3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List all packages:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ conda list
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Install a pacakge:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ conda install numpy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>list environment/ chk out current env</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ conda env list
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Move to an env</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ source activate {env_name}  //on window os
+$ source deactivate {env_name}  //on window os
+$ activate {env_name}  //on bash
+$ deactivate {env_name}  //on bash
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Create env:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$ conda create -n my_env numpy [more-packages...]</t>
+    </r>
+  </si>
+  <si>
+    <t>Install conda</t>
+  </si>
+  <si>
+    <t>Anaconda is an implementation of conda, install it and conda commands can be run.</t>
+  </si>
+  <si>
+    <t>array basic</t>
+  </si>
+  <si>
+    <t>dictionary basic</t>
+  </si>
+  <si>
+    <t>set basic</t>
+  </si>
+  <si>
+    <t>縮句式</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a = [ u for u in v ]  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>equals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for u in v: a.append(u)
+a = [ u + v for u in v for t in u ] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">equals </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">for u in v: for t in u: a.append( u + v )
+a = [ u for u in v if ' A' in u ] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>equlas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for u in v: if ' A' in u: a.append( u )
+p.s. can be used in not only [ ] but ( )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create an array:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a = [ 'A', B', 'C' ]
+$ a = [ x for x in 'ABCD' ]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Add element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a.append( x )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Read element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a[i]
+$ for x in a: print(x)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a[i] = x
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delete an element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ del( a[i] )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create a set:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a = set( […] )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create a dictionary:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a = dict()
+$ a = dict( [ ('A', 1), ('B', 2), ('C', 3) ] )
+$ a = dict( zip( [ 'A', 'B', 'C' ], [ 1, 2, 3 ] ) )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Create an element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a[ newkey ] = initvalue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Read an element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a[ key ]
+$ a.keys()   //show all keys in array
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update an element:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+$ a[ oldkey ] = newvalue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Delete an element:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$ del( a[ oldkey ] )
+p.s. the key of a dictionary cannot be duplicated, will take the last input</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,13 +551,47 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,12 +606,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -440,125 +920,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="66.5" customWidth="1"/>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="66.5" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" ht="25.5" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+    <row r="3" spans="1:3" ht="51">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="4" spans="1:3" ht="114.75">
+      <c r="A4" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="38.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
+    <row r="7" spans="1:3" ht="38.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" ht="153">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
+    <row r="9" spans="1:3" ht="178.5">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
+    <row r="10" spans="1:3" ht="25.5">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="47.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="47.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
+    <row r="11" spans="1:3" ht="51">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A12"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add python entry on range usage
</commit_message>
<xml_diff>
--- a/python.xlsx
+++ b/python.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>/* move the python 101 here */</t>
   </si>
@@ -66,7 +66,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -76,7 +76,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -89,7 +89,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -99,7 +99,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -113,7 +113,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -123,7 +123,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -136,7 +136,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -146,7 +146,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -162,7 +162,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -173,7 +173,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -207,7 +207,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -217,7 +217,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -229,7 +229,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -239,7 +239,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -251,7 +251,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -261,7 +261,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -275,7 +275,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -285,7 +285,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -298,7 +298,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -309,7 +309,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -322,7 +322,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -332,7 +332,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -346,7 +346,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -356,7 +356,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -369,7 +369,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -379,7 +379,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -393,7 +393,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -403,7 +403,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -417,7 +417,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -427,7 +427,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -442,7 +442,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -452,7 +452,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -465,7 +465,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -475,7 +475,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -489,7 +489,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -499,7 +499,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -512,7 +512,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -523,7 +523,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -586,22 +586,31 @@
     print(d)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>## Range usage</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt; for i in range(5):    //print 0,1,2,3,4
+&gt;&gt;&gt; for i in range(3, 6):    //print 3,4,5
+&gt;&gt;&gt; for i in range(4, 10, 2):    //print 4,6,8
+&gt;&gt;&gt; for i in range(0, -10, -2):    //print 0,-2,-4,-6,-8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -609,14 +618,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -624,7 +633,7 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -678,7 +687,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -691,7 +700,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -765,7 +774,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -800,7 +808,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -976,22 +983,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="66.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="66.5" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="51">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="114.75">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1035,12 +1042,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="38.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1051,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="38.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="165.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="153">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1073,7 +1080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="193.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="178.5">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="25.5">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="51">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1113,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="63.75">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1117,7 +1124,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="51">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="73.900000000000006" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="51">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1148,6 +1155,17 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="51">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1158,12 +1176,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1171,12 +1189,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>